<commit_message>
add update to excel data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Documents\Code\JavaScript\excel-to-mongo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\JavaScript\excel-to-mongo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AB78FF-CEE6-4AB5-BC1A-DC14FDB1AB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEFFBB0-1A13-4F19-9B38-F26EA325D7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DBCDF870-5942-4714-9E89-13B949365442}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="34125" windowHeight="13275" xr2:uid="{DBCDF870-5942-4714-9E89-13B949365442}"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
@@ -422,29 +422,29 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -477,7 +477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
remove useless environment variables
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Documents\Code\JavaScript\excel-to-mongo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\JavaScript\excel-to-mongo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF56C1BF-ECEA-481A-AAF3-8DE0B8A03E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B33A7F2-DD13-40B6-B7CF-BA9AF20F5240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DBCDF870-5942-4714-9E89-13B949365442}"/>
+    <workbookView xWindow="5700" yWindow="1470" windowWidth="34125" windowHeight="19230" xr2:uid="{DBCDF870-5942-4714-9E89-13B949365442}"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
@@ -343,9 +343,6 @@
     <t>cell data 100</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>aa</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>gg</t>
+  </si>
+  <si>
+    <t>yearPublished</t>
   </si>
 </sst>
 </file>
@@ -728,20 +728,20 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -749,18 +749,18 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="1">
         <v>1800</v>
@@ -769,12 +769,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1">
         <v>1801</v>
@@ -783,12 +783,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="1">
         <v>1802</v>
@@ -797,12 +797,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1">
         <v>1803</v>
@@ -811,12 +811,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1">
         <v>1804</v>
@@ -825,12 +825,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="1">
         <v>1805</v>
@@ -839,12 +839,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="1">
         <v>1806</v>
@@ -853,12 +853,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="1">
         <v>1807</v>
@@ -867,12 +867,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="1">
         <v>1808</v>
@@ -881,12 +881,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="1">
         <v>1809</v>
@@ -895,12 +895,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1">
         <v>1810</v>
@@ -909,12 +909,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="1">
         <v>1811</v>
@@ -923,12 +923,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="1">
         <v>1812</v>
@@ -937,12 +937,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1">
         <v>1813</v>
@@ -951,12 +951,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1">
         <v>1814</v>
@@ -965,12 +965,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" s="1">
         <v>1815</v>
@@ -979,12 +979,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="1">
         <v>1816</v>
@@ -993,12 +993,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1">
         <v>1817</v>
@@ -1007,12 +1007,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1">
         <v>1818</v>
@@ -1021,12 +1021,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" s="1">
         <v>1819</v>
@@ -1035,12 +1035,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="1">
         <v>1820</v>
@@ -1049,12 +1049,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23" s="1">
         <v>1821</v>
@@ -1063,12 +1063,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="1">
         <v>1822</v>
@@ -1077,12 +1077,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" s="1">
         <v>1823</v>
@@ -1091,12 +1091,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="1">
         <v>1824</v>
@@ -1105,12 +1105,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" s="1">
         <v>1825</v>
@@ -1119,12 +1119,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="1">
         <v>1826</v>
@@ -1133,12 +1133,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="1">
         <v>1827</v>
@@ -1147,12 +1147,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="1">
         <v>1828</v>
@@ -1161,12 +1161,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" s="1">
         <v>1829</v>
@@ -1175,12 +1175,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" s="1">
         <v>1830</v>
@@ -1189,12 +1189,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="1">
         <v>1831</v>
@@ -1203,12 +1203,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="1">
         <v>1832</v>
@@ -1217,12 +1217,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="1">
         <v>1833</v>
@@ -1231,12 +1231,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="1">
         <v>1834</v>
@@ -1245,12 +1245,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1">
         <v>1835</v>
@@ -1259,12 +1259,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="1">
         <v>1836</v>
@@ -1273,12 +1273,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1">
         <v>1837</v>
@@ -1287,12 +1287,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1">
         <v>1838</v>
@@ -1301,12 +1301,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1">
         <v>1839</v>
@@ -1315,12 +1315,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="1">
         <v>1840</v>
@@ -1329,12 +1329,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" s="1">
         <v>1841</v>
@@ -1343,12 +1343,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1">
         <v>1842</v>
@@ -1357,12 +1357,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="1">
         <v>1843</v>
@@ -1371,12 +1371,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C46" s="1">
         <v>1844</v>
@@ -1385,12 +1385,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C47" s="1">
         <v>1845</v>
@@ -1399,12 +1399,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C48" s="1">
         <v>1846</v>
@@ -1413,12 +1413,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" s="1">
         <v>1847</v>
@@ -1427,12 +1427,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1">
         <v>1848</v>
@@ -1441,12 +1441,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1">
         <v>1849</v>
@@ -1455,12 +1455,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1">
         <v>1850</v>
@@ -1469,12 +1469,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" s="1">
         <v>1851</v>
@@ -1483,12 +1483,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54" s="1">
         <v>1852</v>
@@ -1497,12 +1497,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C55" s="1">
         <v>1853</v>
@@ -1511,12 +1511,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C56" s="1">
         <v>1854</v>
@@ -1525,12 +1525,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C57" s="1">
         <v>1855</v>
@@ -1539,12 +1539,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1">
         <v>1856</v>
@@ -1553,12 +1553,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59" s="1">
         <v>1857</v>
@@ -1567,12 +1567,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C60" s="1">
         <v>1858</v>
@@ -1581,12 +1581,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61" s="1">
         <v>1859</v>
@@ -1595,12 +1595,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C62" s="1">
         <v>1860</v>
@@ -1609,12 +1609,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63" s="1">
         <v>1861</v>
@@ -1623,12 +1623,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C64" s="1">
         <v>1862</v>
@@ -1637,12 +1637,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C65" s="1">
         <v>1863</v>
@@ -1651,12 +1651,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C66" s="1">
         <v>1864</v>
@@ -1665,12 +1665,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C67" s="1">
         <v>1865</v>
@@ -1679,12 +1679,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C68" s="1">
         <v>1866</v>
@@ -1693,12 +1693,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C69" s="1">
         <v>1867</v>
@@ -1707,12 +1707,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C70" s="1">
         <v>1868</v>
@@ -1721,12 +1721,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C71" s="1">
         <v>1869</v>
@@ -1735,12 +1735,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C72" s="1">
         <v>1870</v>
@@ -1749,12 +1749,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C73" s="1">
         <v>1871</v>
@@ -1763,12 +1763,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C74" s="1">
         <v>1872</v>
@@ -1777,12 +1777,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="1">
         <v>1873</v>
@@ -1791,12 +1791,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" s="1">
         <v>1874</v>
@@ -1805,12 +1805,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C77" s="1">
         <v>1875</v>
@@ -1819,12 +1819,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C78" s="1">
         <v>1876</v>
@@ -1833,12 +1833,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C79" s="1">
         <v>1877</v>
@@ -1847,12 +1847,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C80" s="1">
         <v>1878</v>
@@ -1861,12 +1861,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C81" s="1">
         <v>1879</v>
@@ -1875,12 +1875,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C82" s="1">
         <v>1880</v>
@@ -1889,12 +1889,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C83" s="1">
         <v>1881</v>
@@ -1903,12 +1903,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C84" s="1">
         <v>1882</v>
@@ -1917,12 +1917,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C85" s="1">
         <v>1883</v>
@@ -1931,12 +1931,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86" s="1">
         <v>1884</v>
@@ -1945,12 +1945,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C87" s="1">
         <v>1885</v>
@@ -1959,12 +1959,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C88" s="1">
         <v>1886</v>
@@ -1973,12 +1973,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C89" s="1">
         <v>1887</v>
@@ -1987,12 +1987,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" s="1">
         <v>1888</v>
@@ -2001,12 +2001,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C91" s="1">
         <v>1889</v>
@@ -2015,12 +2015,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C92" s="1">
         <v>1890</v>
@@ -2029,12 +2029,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C93" s="1">
         <v>1891</v>
@@ -2043,12 +2043,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C94" s="1">
         <v>1892</v>
@@ -2057,12 +2057,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C95" s="1">
         <v>1893</v>
@@ -2071,12 +2071,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C96" s="1">
         <v>1894</v>
@@ -2085,12 +2085,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C97" s="1">
         <v>1895</v>
@@ -2099,12 +2099,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C98" s="1">
         <v>1896</v>
@@ -2113,12 +2113,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C99" s="1">
         <v>1897</v>
@@ -2127,12 +2127,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C100" s="1">
         <v>1898</v>
@@ -2141,12 +2141,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C101" s="1">
         <v>1899</v>

</xml_diff>